<commit_message>
Add note on iOS video.
</commit_message>
<xml_diff>
--- a/FeatureList.xlsx
+++ b/FeatureList.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsdanielson\My Projects\WebApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamoore\Documents\Dev\WebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="17970" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>Web App</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Audio</t>
+  </si>
+  <si>
+    <t>Video on iOS</t>
+  </si>
+  <si>
+    <t>Can take video, can't immediately load and play. Decode error.</t>
   </si>
 </sst>
 </file>
@@ -410,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +631,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add offline column to features.
</commit_message>
<xml_diff>
--- a/FeatureList.xlsx
+++ b/FeatureList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="17970" windowHeight="6135"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="17970" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
   <si>
     <t>Web App</t>
   </si>
@@ -95,10 +95,19 @@
     <t>Audio</t>
   </si>
   <si>
-    <t>Video on iOS</t>
-  </si>
-  <si>
     <t>Can take video, can't immediately load and play. Decode error.</t>
+  </si>
+  <si>
+    <t>Web Video on iOS</t>
+  </si>
+  <si>
+    <t>Web Audio on iOS</t>
+  </si>
+  <si>
+    <t>Offline</t>
+  </si>
+  <si>
+    <t>input type="audio/*" not supported; can take video and strip audio</t>
   </si>
 </sst>
 </file>
@@ -416,10 +425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,9 +439,15 @@
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -480,8 +496,11 @@
       <c r="Q1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -506,11 +525,14 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
       <c r="J2" t="s">
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -530,8 +552,11 @@
       <c r="Q2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -556,6 +581,9 @@
       <c r="H3" t="s">
         <v>4</v>
       </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
       <c r="J3" t="s">
         <v>4</v>
       </c>
@@ -580,8 +608,11 @@
       <c r="Q3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -606,6 +637,9 @@
       <c r="H4" t="s">
         <v>11</v>
       </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
       <c r="J4" t="s">
         <v>4</v>
       </c>
@@ -630,15 +664,28 @@
       <c r="Q4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
-        <v>24</v>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>